<commit_message>
Modelado de datos con  Markdown
</commit_message>
<xml_diff>
--- a/Normalización.xlsx
+++ b/Normalización.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSamu\OneDrive\Documentos\BD - SQL\BD-SQL_Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29329537-A522-4A40-BD57-2AD9C94985C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DB13F1-62D3-4649-B5B8-D0B05749042E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{6362ABD5-D550-47A1-8806-3224D342D6E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{6362ABD5-D550-47A1-8806-3224D342D6E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo Desnormalizado" sheetId="1" r:id="rId1"/>
-    <sheet name="1FN" sheetId="3" r:id="rId2"/>
-    <sheet name="2FN" sheetId="4" r:id="rId3"/>
+    <sheet name="2FN" sheetId="4" r:id="rId2"/>
+    <sheet name="1FN" sheetId="3" r:id="rId3"/>
     <sheet name="2FN-II" sheetId="5" r:id="rId4"/>
     <sheet name="3FN" sheetId="6" r:id="rId5"/>
     <sheet name="4FN" sheetId="8" r:id="rId6"/>
@@ -658,7 +658,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,302 +893,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2707EE7A-94FC-44C5-B783-D2A3BBBC8246}">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:N10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>45292</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="1">
-        <v>918999043</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1">
-        <v>3100</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="4">
-        <v>3000</v>
-      </c>
-      <c r="N2" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>45293</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="1">
-        <v>847776875</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="1">
-        <v>4100</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="4">
-        <v>6000</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>45294</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="1">
-        <v>982761756</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="1">
-        <v>6400</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="4">
-        <v>700</v>
-      </c>
-      <c r="N4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>45295</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="1">
-        <v>938746162</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="1">
-        <v>6400</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="4">
-        <v>3000</v>
-      </c>
-      <c r="N5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>45296</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="1">
-        <v>972647263</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="1">
-        <v>3920</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="4">
-        <v>700</v>
-      </c>
-      <c r="N6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E10" s="6"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{7D627749-3FFC-4AC3-BEF5-74AA59EF7739}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{1CA4E672-8C11-4C71-9B92-CE41693D7D80}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{FEADF71C-8A23-4BA7-ABB0-C4AD3D2C20C4}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{CC3B483B-CB98-4942-AFB6-5D2BF83B0568}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{1F2ED31E-BDBB-4071-8007-83B1A9408AD2}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F1B056-157A-483A-AEB5-C87EBFE28F7C}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -1518,6 +1222,302 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2707EE7A-94FC-44C5-B783-D2A3BBBC8246}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45292</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1">
+        <v>918999043</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1">
+        <v>3100</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="4">
+        <v>3000</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45293</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1">
+        <v>847776875</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4100</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="4">
+        <v>6000</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45294</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1">
+        <v>982761756</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1">
+        <v>6400</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="4">
+        <v>700</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45295</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="1">
+        <v>938746162</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1">
+        <v>6400</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="4">
+        <v>3000</v>
+      </c>
+      <c r="N5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45296</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1">
+        <v>972647263</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3920</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="4">
+        <v>700</v>
+      </c>
+      <c r="N6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E10" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{7D627749-3FFC-4AC3-BEF5-74AA59EF7739}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{1CA4E672-8C11-4C71-9B92-CE41693D7D80}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{FEADF71C-8A23-4BA7-ABB0-C4AD3D2C20C4}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{CC3B483B-CB98-4942-AFB6-5D2BF83B0568}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{1F2ED31E-BDBB-4071-8007-83B1A9408AD2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F252ED24-5F91-4414-B5C2-2A594212F0A3}">
   <sheetPr>
@@ -1526,7 +1526,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="A1:O13"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,8 +1874,8 @@
   </sheetPr>
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2224,7 +2224,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J13" s="6"/>
+      <c r="J13" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2243,7 +2243,7 @@
   </sheetPr>
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" activeCellId="2" sqref="J8 I9 H7"/>
     </sheetView>
   </sheetViews>
@@ -2478,7 +2478,6 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H7" s="11"/>
       <c r="L7" s="7" t="s">
         <v>5</v>
       </c>
@@ -2502,7 +2501,6 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J8" s="11"/>
       <c r="L8">
         <v>1</v>
       </c>
@@ -2526,7 +2524,6 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I9" s="11"/>
       <c r="L9">
         <v>2</v>
       </c>

</xml_diff>